<commit_message>
Added some sfx to FMOD
</commit_message>
<xml_diff>
--- a/documentation/assets.xlsx
+++ b/documentation/assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camso\Documents\School\Game Audio\Final\Game-Audio-Final\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627CF933-C629-4AC3-B62F-4CC864FF0BF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD15B34-8416-46F6-BF65-5C707FBFFCB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Asset Name</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>FMOD started</t>
-  </si>
-  <si>
-    <t>Recording</t>
   </si>
 </sst>
 </file>
@@ -612,7 +609,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -661,8 +658,8 @@
       <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>8</v>
+      <c r="F2" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
@@ -682,7 +679,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
All planned effects added to game
</commit_message>
<xml_diff>
--- a/documentation/assets.xlsx
+++ b/documentation/assets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camso\Documents\School\Game Audio\Final\Game-Audio-Final\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C927773-BDAE-4713-8B18-97511266FA2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D1CBA2-8FAF-44ED-B1D8-8D6961A5674D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Asset Name</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Sound of thrusters burning and propelling a ship forward</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>Thruster noise, fire/torch</t>
   </si>
   <si>
@@ -177,27 +174,17 @@
     <t>1 Complete</t>
   </si>
   <si>
-    <t>Recorded</t>
-  </si>
-  <si>
-    <t>FMOD Started</t>
+    <t>(Tentatively) Complete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,35 +199,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -257,16 +227,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -275,26 +243,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Good" xfId="3" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -635,7 +595,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -655,14 +615,14 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>46</v>
+      <c r="E1" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -670,122 +630,122 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>49</v>
+      <c r="F2" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="E3" s="4">
         <v>2</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>51</v>
+      <c r="F3" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="E4" s="4">
         <v>2</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>50</v>
+      <c r="F4" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>49</v>
+      <c r="E5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="E6" s="4">
         <v>1</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>8</v>
+      <c r="F6" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>48</v>
+      <c r="F7" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
@@ -793,119 +753,119 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>48</v>
+      <c r="F8" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="E9" s="4">
         <v>2</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>50</v>
+      <c r="F9" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>8</v>
+      <c r="F10" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>8</v>
+      <c r="F11" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>8</v>
+      <c r="F12" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="E13" s="4">
         <v>1</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>8</v>
+      <c r="F13" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>